<commit_message>
Orangehrm site till 4 test cases
</commit_message>
<xml_diff>
--- a/TestcaseOrangeHRM.xlsx
+++ b/TestcaseOrangeHRM.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="66" documentId="8_{2E0A0D5A-FB4E-4CD7-B77F-BFD54E4E9662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF94E543-581F-4F2D-A31B-A8F5580EB11E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E268510E-E7EF-4177-9496-93435FAB452B}"/>
+    <workbookView minimized="1" xWindow="6108" yWindow="3708" windowWidth="17280" windowHeight="8880" xr2:uid="{E268510E-E7EF-4177-9496-93435FAB452B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -783,6 +783,9 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -791,9 +794,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1147,8 +1147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB2069E3-5B59-4449-8F28-2034C8C7B723}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="53" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="59" zoomScaleNormal="53" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1170,52 +1170,52 @@
       <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="20"/>
     </row>
     <row r="2" spans="2:12">
       <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="20"/>
     </row>
     <row r="3" spans="2:12">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="17" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="20"/>
     </row>
     <row r="4" spans="2:12">
       <c r="B4" s="16" t="s">
@@ -1239,15 +1239,15 @@
       <c r="C5" s="25">
         <v>45921</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="20"/>
     </row>
     <row r="7" spans="2:12" ht="15" thickBot="1"/>
     <row r="8" spans="2:12" ht="15.6">
@@ -1625,7 +1625,7 @@
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:12" ht="83.4">
+    <row r="20" spans="1:12" ht="69.599999999999994">
       <c r="A20" s="13"/>
       <c r="B20" s="4">
         <v>12</v>

</xml_diff>